<commit_message>
super new update with cronjob for payment gateway and Digiwallet integration
</commit_message>
<xml_diff>
--- a/public/assets/items_bulk_format_nodata.xlsx
+++ b/public/assets/items_bulk_format_nodata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Variations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChoiceOptions</t>
   </si>
   <si>
     <t xml:space="preserve">AddOns</t>
@@ -184,15 +187,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U106"/>
+  <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -256,6 +259,9 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -278,6 +284,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
@@ -300,6 +307,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
@@ -314,12 +322,12 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -334,12 +342,12 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -354,14 +362,12 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="V6" s="1"/>
+    </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
@@ -375,11 +381,11 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
@@ -394,12 +400,12 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
@@ -414,11 +420,11 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
@@ -433,12 +439,12 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
@@ -453,12 +459,12 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
@@ -473,13 +479,13 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
@@ -494,12 +500,12 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
@@ -514,12 +520,12 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
@@ -534,11 +540,11 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
@@ -553,11 +559,11 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
@@ -572,13 +578,13 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
@@ -593,11 +599,11 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
@@ -612,13 +618,13 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
@@ -633,11 +639,11 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
@@ -652,13 +658,13 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
@@ -673,11 +679,11 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
@@ -692,12 +698,12 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
@@ -712,11 +718,11 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
@@ -731,13 +737,13 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
@@ -752,13 +758,13 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
@@ -773,11 +779,11 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
@@ -792,13 +798,13 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
@@ -813,12 +819,12 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
@@ -833,11 +839,11 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
@@ -854,11 +860,12 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="O33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
@@ -873,13 +880,13 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
@@ -894,12 +901,12 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="P35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
@@ -914,12 +921,12 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
@@ -934,11 +941,11 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
@@ -953,12 +960,12 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="P38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
@@ -973,11 +980,11 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
@@ -992,11 +999,11 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
@@ -1011,11 +1018,11 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
@@ -1030,12 +1037,12 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="Q42" s="1"/>
+      <c r="P42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
@@ -1050,13 +1057,13 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-      <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
@@ -1071,13 +1078,13 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
@@ -1092,12 +1099,12 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="P45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
@@ -1112,11 +1119,11 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
@@ -1131,12 +1138,12 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="P47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
@@ -1151,12 +1158,12 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="P48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
@@ -1171,11 +1178,11 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
@@ -1190,11 +1197,11 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
@@ -1209,12 +1216,12 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="P51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
@@ -1229,12 +1236,12 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="P52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
@@ -1249,11 +1256,11 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
@@ -1268,11 +1275,11 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
@@ -1287,11 +1294,11 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
@@ -1306,12 +1313,12 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
@@ -1326,11 +1333,11 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-      <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
@@ -1345,13 +1352,13 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
-      <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
@@ -1366,12 +1373,12 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
-      <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
@@ -1386,11 +1393,11 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
-      <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
@@ -1413,6 +1420,7 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
@@ -1427,13 +1435,13 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
@@ -1448,13 +1456,13 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
-      <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1"/>
@@ -1469,12 +1477,12 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1"/>
@@ -1490,11 +1498,12 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
-      <c r="Q65" s="1"/>
+      <c r="O65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1"/>
@@ -1509,12 +1518,12 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="Q66" s="1"/>
+      <c r="P66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1"/>
@@ -1529,12 +1538,12 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="Q67" s="1"/>
+      <c r="P67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
@@ -1549,11 +1558,11 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
-      <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
@@ -1568,11 +1577,11 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
-      <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
@@ -1587,12 +1596,12 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="Q70" s="1"/>
+      <c r="P70" s="1"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
@@ -1607,12 +1616,12 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="Q71" s="1"/>
+      <c r="P71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1"/>
@@ -1627,12 +1636,12 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="Q72" s="1"/>
+      <c r="P72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
@@ -1647,12 +1656,12 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="Q73" s="1"/>
+      <c r="P73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1"/>
@@ -1667,12 +1676,12 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="Q74" s="1"/>
+      <c r="P74" s="1"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
@@ -1687,12 +1696,12 @@
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="Q75" s="1"/>
+      <c r="P75" s="1"/>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1"/>
@@ -1707,12 +1716,12 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="Q76" s="1"/>
+      <c r="P76" s="1"/>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1"/>
@@ -1727,12 +1736,12 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="Q77" s="1"/>
+      <c r="P77" s="1"/>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1"/>
@@ -1747,11 +1756,11 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
-      <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1"/>
@@ -1766,12 +1775,12 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="Q79" s="1"/>
+      <c r="P79" s="1"/>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
@@ -1786,11 +1795,11 @@
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
-      <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
@@ -1805,11 +1814,11 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
-      <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
@@ -1824,11 +1833,11 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1"/>
@@ -1843,12 +1852,12 @@
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
-      <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1"/>
@@ -1863,12 +1872,12 @@
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
-      <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
@@ -1883,12 +1892,12 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
-      <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
@@ -1904,12 +1913,12 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1"/>
@@ -1924,12 +1933,12 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
-      <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
@@ -1944,12 +1953,12 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
-      <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1"/>
@@ -1964,12 +1973,12 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
-      <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
@@ -1984,11 +1993,11 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
-      <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1"/>
@@ -2003,11 +2012,11 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
-      <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1"/>
@@ -2022,11 +2031,11 @@
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
-      <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1"/>
@@ -2041,11 +2050,11 @@
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
-      <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1"/>
@@ -2060,12 +2069,12 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
-      <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
@@ -2080,12 +2089,12 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
-      <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1"/>
@@ -2100,11 +2109,11 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
-      <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
@@ -2119,11 +2128,11 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
-      <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
@@ -2139,12 +2148,12 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="Q98" s="1"/>
+      <c r="P98" s="1"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
@@ -2159,11 +2168,11 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
-      <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
@@ -2179,11 +2188,11 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
-      <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
@@ -2199,12 +2208,12 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="Q101" s="1"/>
+      <c r="P101" s="1"/>
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1"/>
@@ -2220,13 +2229,13 @@
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
-      <c r="O102" s="1"/>
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1"/>
@@ -2242,11 +2251,11 @@
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
-      <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1"/>
@@ -2263,11 +2272,12 @@
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
-      <c r="Q104" s="1"/>
+      <c r="O104" s="1"/>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
@@ -2285,11 +2295,12 @@
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
-      <c r="Q105" s="1"/>
+      <c r="P105" s="1"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
@@ -2305,11 +2316,12 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
-      <c r="Q106" s="1"/>
+      <c r="O106" s="1"/>
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>